<commit_message>
Added "Bloodstained Chivalry" data into ArtifactSetTable.xlsx
</commit_message>
<xml_diff>
--- a/data/ArtifactSetTable.xlsx
+++ b/data/ArtifactSetTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\GenshinSim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9512FD6C-97AD-4ED5-BD6A-D7FF41377B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289883EA-24C0-480E-9C0B-7CD30F24D1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ArtifactSetDataTable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>### FIELD_NAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +55,17 @@
 [StatisticBoost;DamageModifier_PhysicalDamage=0.25;],
 ,
 [StatisticBoost,Stackable;Attack_Percentage=0.09,MaxNumStacks=0,InitialNumStacks=0;,StatisticBoost,Triggerable;DamageModifier_PhysicalDamage=0.25;],</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bloodstained Chivalry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,
+[StatisticBoost;DamageModifier_PhysicalDamage=0.25;],
+,
+[StatisticBoost,Triggerable;DamageModifier_ChargedAttack=0.25;],</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -386,17 +397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="132.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="135.5" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -425,6 +436,14 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>